<commit_message>
made changes to "Date" and "Format-Extent" fields
- added "circa date" example to "Date" field
- added "dimensions" example to "Format-Extent" field
</commit_message>
<xml_diff>
--- a/data dictionary/dataDictionary.xlsx
+++ b/data dictionary/dataDictionary.xlsx
@@ -5,18 +5,68 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtshelby\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtshelby\Box Sync\iastate\DARCTeam\digitalCollections\github_resources\dataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="888" yWindow="0" windowWidth="22152" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Core" sheetId="1" r:id="rId1"/>
     <sheet name="Additional" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="additionalFieldTextTable_dataImportIntoExcel" localSheetId="1">Additional!$A$1:$K$17</definedName>
+    <definedName name="coreFieldTextTable_dataImportIntoExcel" localSheetId="0">Core!$A$1:$K$19</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="additionalFieldTextTable_dataImportIntoExcel" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jtshelby\Box Sync\iastate\DARCTeam\digitalCollections\github_resources\dataDictionary\additionalFieldTextTable_dataImportIntoExcel.txt" tab="0" delimiter="|">
+      <textFields count="12">
+        <textField type="skip"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="coreFieldTextTable_dataImportIntoExcel" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\jtshelby\Box Sync\iastate\DARCTeam\digitalCollections\github_resources\dataDictionary\coreFieldTextTable_dataImportIntoExcel.txt" delimiter="|">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,7 +96,7 @@
     <t xml:space="preserve"> Guidelines (including sources of information, encoding vocabularies used...)                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Example                                                                                                                                                                                                                                                                                                                                                                                                                          </t>
+    <t xml:space="preserve"> Example                                                                                                                                                                                                                                                                                                                                                                                                                                </t>
   </si>
   <si>
     <t xml:space="preserve"> Who creates values                                                                                    </t>
@@ -76,7 +126,7 @@
     <t xml:space="preserve"> Use the call number assigned by Special Collections, University Archives, Cataloging and Metadata Unit, or other similar authority. Follow formatting given in the original resource.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> RS 9/7/11 Box 40                                                                                                                                                                                                                                                                                                                                                                                                                 </t>
+    <t xml:space="preserve"> RS 9/7/11 Box 40                                                                                                                                                                                                                                                                                                                                                                                                                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Digital Initiatives staff or metadata librarian enter values assigned by Special Collections          </t>
@@ -94,7 +144,7 @@
     <t xml:space="preserve"> The physical collection to which the items belong in the library collection. This may or may not be the same for all items in a collection. Use a colon (:) to separate the collection name and URL.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                         </t>
   </si>
   <si>
-    <t xml:space="preserve"> Jay Brownlee Davidson (1880-1957) Papers, 1905-2005, undated: [http://www.add.lib.iastate.edu/spcl/arch/rgrp/9-7-11.pdf](http://www.add.lib.iastate.edu/spcl/arch/rgrp/9-7-11.pdf)                                                                                                                                                                                                                                               </t>
+    <t xml:space="preserve"> Jay Brownlee Davidson (1880-1957) Papers, 1905-2005, undated: [http://www.add.lib.iastate.edu/spcl/arch/rgrp/9-7-11.pdf](http://www.add.lib.iastate.edu/spcl/arch/rgrp/9-7-11.pdf)                                                                                                                                                                                                                                                     </t>
   </si>
   <si>
     <t xml:space="preserve"> Contributing Institution </t>
@@ -115,7 +165,7 @@
     <t xml:space="preserve"> The primary value will always be *Iowa State University Library Special Collections: [http://www.add.lib.iastate.edu/spcl/index.html](http://www.add.lib.iastate.edu/spcl/index.html)*. If an external entity shares responsibility, add their location afterwards, following a semicolon (;).                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                               </t>
   </si>
   <si>
-    <t xml:space="preserve"> Iowa State University Library Special Collections: [http://www.add.lib.iastate.edu/spcl/index.html](http://www.add.lib.iastate.edu/spcl/index.html)  &lt;br&gt;&lt;br&gt;  Iowa State University Library Special Collections: [http://www.add.lib.iastate.edu/spcl/index.html](http://www.add.lib.iastate.edu/spcl/index.html); International Textile and Apparel,Association: [http://www.itaaonline.org/](http://www.itaaonline.org/)      </t>
+    <t xml:space="preserve"> Iowa State University Library Special Collections: [http://www.add.lib.iastate.edu/spcl/index.html](http://www.add.lib.iastate.edu/spcl/index.html)  &lt;br&gt;&lt;br&gt;  Iowa State University Library Special Collections: [http://www.add.lib.iastate.edu/spcl/index.html](http://www.add.lib.iastate.edu/spcl/index.html); International Textile and Apparel,Association: [http://www.itaaonline.org/](http://www.itaaonline.org/)            </t>
   </si>
   <si>
     <t xml:space="preserve"> Digital Initiatives staff or metadata librarian enter values per information from Special Collections </t>
@@ -139,7 +189,7 @@
     <t xml:space="preserve"> Use values in the local controlled vocabulary or Library of Congress Name Authorities to identify the given creator(s) of the resource. For images of creative works (such as photographs of statues), the creator of the photograph as well as of the creative work pictured may both be included, if known.  &lt;br&gt;&lt;br&gt;  If creator cannot be determined, leave blank.                                                                                                                                                                                                                                                                                                                                                                                                                                                                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> Davidson, Jay Brownlee (1880-1957)  &lt;br&gt;&lt;br&gt;  II International Congress on Rural Engineering, Madrid, Spain, 1935  &lt;br&gt;&lt;br&gt;   *[blank value]*                                                                                                                                                                                                                                                                                    </t>
+    <t xml:space="preserve"> Davidson, Jay Brownlee (1880-1957)  &lt;br&gt;&lt;br&gt;  II International Congress on Rural Engineering, Madrid, Spain, 1935  &lt;br&gt;&lt;br&gt;   *[blank value]*                                                                                                                                                                                                                                                                                          </t>
   </si>
   <si>
     <t xml:space="preserve"> Cataloging &amp; Metadata Unit                                                                            </t>
@@ -163,7 +213,7 @@
     <t xml:space="preserve"> Use the ISO 8601 date format (yyyy-mm-dd).  &lt;br&gt;&lt;br&gt;  Do not use abbreviations such as c. or n.d.  &lt;br&gt;&lt;br&gt;  Use yyyy - yyyy for range. If date range cannot be determined or narrowed at all leave blank.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                   </t>
   </si>
   <si>
-    <t xml:space="preserve"> Known year-month-day: 2001-10-19  &lt;br&gt;&lt;br&gt;  Known year-month: 2001-10  &lt;br&gt;&lt;br&gt;  Known year: 2001  &lt;br&gt;&lt;br&gt;  One year or another: 1892 or 1893  &lt;br&gt;&lt;br&gt;  Circa year: 1892  &lt;br&gt;&lt;br&gt;  Decade certain: 1970s; 1965 - 1975 (spaces around hyphen)  &lt;br&gt;&lt;br&gt;  Uncertain range: 1965? - 1975?  &lt;br&gt;&lt;br&gt;  Before a time period: Before 1867  &lt;br&gt;&lt;br&gt;  After a time period: After 1867  &lt;br&gt;&lt;br&gt;  Completely unknown: *[blank value]* </t>
+    <t xml:space="preserve"> Known year-month-day: 2001-10-19  &lt;br&gt;&lt;br&gt;  Known year-month: 2001-10  &lt;br&gt;&lt;br&gt;  Known year: 2001  &lt;br&gt;&lt;br&gt;  One year or another: 1892 or 1893  &lt;br&gt;&lt;br&gt;  Circa year: circa 1892  &lt;br&gt;&lt;br&gt;  Decade certain: 1970s; 1965 - 1975 (spaces around hyphen)  &lt;br&gt;&lt;br&gt;  Uncertain range: 1965? - 1975?  &lt;br&gt;&lt;br&gt;  Before a time period: Before 1867  &lt;br&gt;&lt;br&gt;  After a time period: After 1867  &lt;br&gt;&lt;br&gt;  Completely unknown: *[blank value]* </t>
   </si>
   <si>
     <t xml:space="preserve"> Date Digital             </t>
@@ -178,7 +228,7 @@
     <t xml:space="preserve"> Use the ISO 8601 date format (yyyy-mm-dd).  &lt;br&gt;&lt;br&gt;  If just a year given, use YYYY.  &lt;br&gt;&lt;br&gt;  Do not use abbreviations such as c. or n.d.  &lt;br&gt;&lt;br&gt;  Use data embedded in the file to determine date digitized. ("Properties")                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                            </t>
   </si>
   <si>
-    <t xml:space="preserve"> 2013-05-13  &lt;br&gt;&lt;br&gt;  2013-06-11                                                                                                                                                                                                                                                                                                                                                                                                 </t>
+    <t xml:space="preserve"> 2013-05-13  &lt;br&gt;&lt;br&gt;  2013-06-11                                                                                                                                                                                                                                                                                                                                                                                                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Digital Initiatives staff or metadata librarian                                                       </t>
@@ -196,7 +246,7 @@
     <t xml:space="preserve"> Construct a brief description of the item using the information found in the finding aid, the MARC record, the item itself, any other documentation accompanying the collection, or context from other sources. Consultation with archival staff may be necessary. For other collections, subject specialists from selected departments may be invited to assist with item description where appropriate.                                                                                                                                                                                                                                                                                                                                                                                                                                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> The Cenotaphy and World War monument, London, 1935.  &lt;br&gt;&lt;br&gt;  Steamboat passengers play shuffleboard on the shipâ€™s deck, 1935.                                                                                                                                                                                                                                                                                                  </t>
+    <t xml:space="preserve"> The Cenotaphy and World War monument, London, 1935.  &lt;br&gt;&lt;br&gt;  Steamboat passengers play shuffleboard on the shipâ€™s deck, 1935.                                                                                                                                                                                                                                                                                                        </t>
   </si>
   <si>
     <t xml:space="preserve"> File Name                </t>
@@ -214,7 +264,7 @@
     <t xml:space="preserve"> Use the filename of the object as it appears in the "ready for catalogers" folder on the Y: drive.  &lt;br&gt;&lt;br&gt;  This should conform to the local identifier construction guidelines.  &lt;br&gt;&lt;br&gt;  For compound objects (for example, a multi-page document or an interview with an accompanying audio track), each component of the compound object should have file name data added, and no file name should be recorded for the compound object as a whole unless appropriate in a special case.                                                                                                                                                                                                                                                                                                                                               </t>
   </si>
   <si>
-    <t xml:space="preserve"> 09-07-11_Davidson_39-01.pdf  &lt;br&gt;&lt;br&gt;  09-07-11_Davidson_40-01.pdf                                                                                                                                                                                                                                                                                                                                                               </t>
+    <t xml:space="preserve"> 09-07-11_Davidson_39-01.pdf  &lt;br&gt;&lt;br&gt;  09-07-11_Davidson_40-01.pdf                                                                                                                                                                                                                                                                                                                                                                     </t>
   </si>
   <si>
     <t xml:space="preserve"> File Type                </t>
@@ -232,7 +282,7 @@
     <t xml:space="preserve"> Values are listed under the Template column in the [IMT](http://www.iana.org/assignments/media-types/media-types.xhtml) vocabulary                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </t>
   </si>
   <si>
-    <t xml:space="preserve"> application/pdf  &lt;br&gt;&lt;br&gt;  image/jpeg                                                                                                                                                                                                                                                                                                                                                                                            </t>
+    <t xml:space="preserve"> application/pdf  &lt;br&gt;&lt;br&gt;  image/jpeg                                                                                                                                                                                                                                                                                                                                                                                                  </t>
   </si>
   <si>
     <t xml:space="preserve"> Format-Extent            </t>
@@ -247,7 +297,7 @@
     <t xml:space="preserve"> Use separate values for each aspect of extent recorded. For multi-page documents, include number of pages. For objects, include dimensions only if given and if they are relevant to the use of the collection. When recording dimensions, use the metric system. For sound or video resources, include time duration of recording.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          </t>
   </si>
   <si>
-    <t xml:space="preserve"> 200 pages  &lt;br&gt;&lt;br&gt;  4 photographs + handwritten notes                                                                                                                                                                                                                                                                                                                                                                           </t>
+    <t xml:space="preserve"> 200 pages  &lt;br&gt;&lt;br&gt;  4 photographs + handwritten notes  &lt;br&gt;&lt;br&gt;  24.2 x 25 cm                                                                                                                                                                                                                                                                                                                                                         </t>
   </si>
   <si>
     <t xml:space="preserve"> Format-Medium            </t>
@@ -262,7 +312,7 @@
     <t xml:space="preserve"> Describe the physical medium of the original (depicted or scanned) resource. Use the local controlled vocabulary which has been derived from the Art and Architecture Thesaurus (AAT), [http://www.getty.edu/research/tools/vocabularies/aat/](http://www.getty.edu/research/tools/vocabularies/aat/). This value should reflect a cultural heritage vocabulary for artifacts rather than an internet media or file type. Use the **preferred** term.                                                                                                                                                                                                                                                                                                                                                                                        </t>
   </si>
   <si>
-    <t xml:space="preserve"> scrapbooks  &lt;br&gt;&lt;br&gt;  albums (books)  &lt;br&gt;&lt;br&gt;  photographs  &lt;br&gt;&lt;br&gt;  portraits  &lt;br&gt;&lt;br&gt;  clippings (information artifacts)  &lt;br&gt;&lt;br&gt;  maps (documents)  &lt;br&gt;&lt;br&gt;  picture postcards  &lt;br&gt;&lt;br&gt;  notes cards (information artifacts)  &lt;br&gt;&lt;br&gt;  business cards  &lt;br&gt;&lt;br&gt;  proceedings  &lt;br&gt;&lt;br&gt;  charts (graphic documents)                                                                                                     </t>
+    <t xml:space="preserve"> scrapbooks  &lt;br&gt;&lt;br&gt;  albums (books)  &lt;br&gt;&lt;br&gt;  photographs  &lt;br&gt;&lt;br&gt;  portraits  &lt;br&gt;&lt;br&gt;  clippings (information artifacts)  &lt;br&gt;&lt;br&gt;  maps (documents)  &lt;br&gt;&lt;br&gt;  picture postcards  &lt;br&gt;&lt;br&gt;  notes cards (information artifacts)  &lt;br&gt;&lt;br&gt;  business cards  &lt;br&gt;&lt;br&gt;  proceedings  &lt;br&gt;&lt;br&gt;  charts (graphic documents)                                                                                                           </t>
   </si>
   <si>
     <t xml:space="preserve"> Identifier (DOI)         </t>
@@ -280,7 +330,7 @@
     <t xml:space="preserve"> Identifiers are assigned using the Digital Object Identifier (DOI) Naming Guidelines (see Appendix V). These should be created at the time of digitization.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                  </t>
   </si>
   <si>
-    <t xml:space="preserve"> 09-07-11_Davidson_39-01  &lt;br&gt;&lt;br&gt;  09-07-11_Davidson_40-01                                                                                                                                                                                                                                                                                                                                                                       </t>
+    <t xml:space="preserve"> 09-07-11_Davidson_39-01  &lt;br&gt;&lt;br&gt;  09-07-11_Davidson_40-01                                                                                                                                                                                                                                                                                                                                                                             </t>
   </si>
   <si>
     <t xml:space="preserve"> Index Date               </t>
@@ -292,7 +342,7 @@
     <t xml:space="preserve"> Use the ISO 8601 date format (yyyy-mm-dd).  &lt;br&gt;&lt;br&gt;  Do not use abbreviations such as c. or n.d.  &lt;br&gt;&lt;br&gt;  For date ranges of ten years or less, list out each date in the range as follow: yyyy yyyy yyyy yyyy  &lt;br&gt;&lt;br&gt;  For date ranges that span more than ten years, follow the guidelines for `Date`                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> For 1870 - 1877: 1870 1871 1872 1873 1874 1875 1876 1877  &lt;br&gt;&lt;br&gt;  For circa 1892: 1890 1891 1892 1893 1894 (two below and two above)                                                                                                                                                                                                                                                                                           </t>
+    <t xml:space="preserve"> For 1870 - 1877: 1870 1871 1872 1873 1874 1875 1876 1877  &lt;br&gt;&lt;br&gt;  For circa 1892: 1890 1891 1892 1893 1894 (two below and two above)                                                                                                                                                                                                                                                                                                 </t>
   </si>
   <si>
     <t xml:space="preserve"> Language                 </t>
@@ -313,7 +363,7 @@
     <t xml:space="preserve"> Use the three letter code indicated by [ISO 693-3](http://www-01.sil.org/iso639-3/codes.asp?order=reference_name).                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </t>
   </si>
   <si>
-    <t xml:space="preserve"> *Letter written in English:* eng &lt;br&gt;&lt;br&gt; *Image of a page of a book written primarily in English but has some French:* eng; fra                                                                                                                                                                                                                                                                                                 </t>
+    <t xml:space="preserve"> *Letter written in English:* eng &lt;br&gt;&lt;br&gt; *Image of a page of a book written primarily in English but has some French:* eng; fra                                                                                                                                                                                                                                                                                                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Rights                   </t>
@@ -328,7 +378,7 @@
     <t xml:space="preserve"> Use statement in accordance with documented institutional and national policies, and in accordance with the stated goals of the project.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                     </t>
   </si>
   <si>
-    <t xml:space="preserve"> U.S. and international copyright laws protect this digital image. Commercial use or distribution of the image is not permitted without prior permission of the copyright holder. For permission to use the digital image, please contact Iowa State University Library Special Collections at archives@iastate.edu. For reproductions see: http://www.add.lib.iastate.edu/spcl/services/photfees.html                            </t>
+    <t xml:space="preserve"> U.S. and international copyright laws protect this digital image. Commercial use or distribution of the image is not permitted without prior permission of the copyright holder. For permission to use the digital image, please contact Iowa State University Library Special Collections at archives@iastate.edu. For reproductions see: http://www.add.lib.iastate.edu/spcl/services/photfees.html                                  </t>
   </si>
   <si>
     <t xml:space="preserve"> Subject                  </t>
@@ -346,7 +396,7 @@
     <t xml:space="preserve"> Select subject headings after performing subject analysis. Use LCSH or local controlled vocabulary as appropriate. Include any personal name, corporate body, or uniform title subjects here as well.  &lt;br&gt;&lt;br&gt;  Do not use full strings for places in this field; instead, enter these in the `Geographic Subject` field, which is mapped to `DC:subject` for Primo and OAI harvesting.  &lt;br&gt;&lt;br&gt;  Use information given in tables of contents within the resource as well as any notes on the object itself; however, it is not obligatory to perform more extensive research for subject analysis beyond what has been included. It is acceptable to include subject terms outside of the controlled vocabularies for the purpose of improving the user search experience. These values will be added to the local controlled vocabulary. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Davidson, J. Brownlee (Jay Brownlee), 1880-1957  &lt;br&gt;&lt;br&gt;  Photographs  &lt;br&gt;&lt;br&gt;  Agricultural engineering--Iowa  &lt;br&gt;&lt;br&gt;  International Harvester Company  &lt;br&gt;&lt;br&gt;  American Society of Agricultural Engineers  &lt;br&gt;&lt;br&gt;  Agricultural machinery  &lt;br&gt;&lt;br&gt;  McKensie,Estelle                                                                                                                                                  </t>
+    <t xml:space="preserve"> Davidson, J. Brownlee (Jay Brownlee), 1880-1957  &lt;br&gt;&lt;br&gt;  Photographs  &lt;br&gt;&lt;br&gt;  Agricultural engineering--Iowa  &lt;br&gt;&lt;br&gt;  International Harvester Company  &lt;br&gt;&lt;br&gt;  American Society of Agricultural Engineers  &lt;br&gt;&lt;br&gt;  Agricultural machinery  &lt;br&gt;&lt;br&gt;  McKensie,Estelle                                                                                                                                                        </t>
   </si>
   <si>
     <t xml:space="preserve"> Title                    </t>
@@ -361,7 +411,7 @@
     <t xml:space="preserve"> Create a descriptive title for the item/object following the general guidelines for titles given in Describing Archives: a Content Standard (DACS) 2.3 Title (page 17).  &lt;br&gt;&lt;br&gt;  Prefer any information given within the resource itself, such as the authorâ€™s table of contents or a hand-written note on an album page serving the function of a title page. Information from the finding aid (see Appendix I) can,also be used to assist in item identification.   &lt;br&gt;&lt;br&gt;  For correspondence, follow the format: **[authorized name of sender] letter to [authorized name of recipient] regarding [subject], [date]**                                                                                                                                                                                                                </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.B. Davidson pictorial record, trip to Europe (Germany, England, France, Spain), book 1 of 3 *[compound object based on hand-written note on title page]*  &lt;br&gt;&lt;br&gt;  J.B. Davidson notes, photographs, and proceedings documenting agricultural work in China, 1948-1949  &lt;br&gt;&lt;br&gt;  Page 6 *[page-level description of compound object]*                                                                                        </t>
+    <t xml:space="preserve"> J.B. Davidson pictorial record, trip to Europe (Germany, England, France, Spain), book 1 of 3 *[compound object based on hand-written note on title page]*  &lt;br&gt;&lt;br&gt;  J.B. Davidson notes, photographs, and proceedings documenting agricultural work in China, 1948-1949  &lt;br&gt;&lt;br&gt;  Page 6 *[page-level description of compound object]*                                                                                              </t>
   </si>
   <si>
     <t xml:space="preserve"> Type                     </t>
@@ -379,7 +429,7 @@
     <t xml:space="preserve"> Use the DCMI Type Vocabulary: [http://dublincore.org/documents/2012/06/14/dcmi-terms/?v=dcmitype#H7](http://dublincore.org/documents/2012/06/14/dcmi-terms/?v=dcmitype#H7). Use the Label instead of the Term Name.  &lt;br&gt;&lt;br&gt;  Describe the overall nature of the item as a human user would perceive it. For example, even if you have a scanned image of a page of a letter, the type would be "Text", not "Image." If the item is a textual object with an image (ex. letter with illustration), the type can be both "Text" and "Image" separated by a semicolon (;).                                                                                                                                                                                                                                                                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> *Image of a page of a letter:* Text &lt;br&gt;&lt;br&gt; *Image of a page of a letter that has an illustration:* Text; Image                                                                                                                                                                                                                                                                                                                 </t>
+    <t xml:space="preserve"> *Image of a page of a letter:* Text &lt;br&gt;&lt;br&gt; *Image of a page of a letter that has an illustration:* Text; Image                                                                                                                                                                                                                                                                                                                       </t>
   </si>
   <si>
     <t xml:space="preserve"> Field label            </t>
@@ -638,7 +688,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,316 +696,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -963,204 +713,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1173,6 +734,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="coreFieldTextTable_dataImportIntoExcel" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="additionalFieldTextTable_dataImportIntoExcel" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1441,13 +1010,17 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="72" customWidth="1"/>
-    <col min="7" max="7" width="51.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="80.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -2060,6 +1633,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2068,10 +1642,20 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="71.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
moved "types of people" from "People" to "Subject"
</commit_message>
<xml_diff>
--- a/data dictionary/dataDictionary.xlsx
+++ b/data dictionary/dataDictionary.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtshelby\Box Sync\iastate\DARCTeam\digitalCollections\github_resources\dataDictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="888" yWindow="0" windowWidth="22152" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Core" sheetId="1" r:id="rId1"/>
     <sheet name="Additional" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="additional" localSheetId="1">Additional!$A$1:$K$17</definedName>
-    <definedName name="core" localSheetId="0">Core!$A$1:$K$19</definedName>
+    <definedName name="excelAdditional." localSheetId="1">Additional!$A$1:$K$17</definedName>
+    <definedName name="excelCore." localSheetId="0">Core!$A$1:$K$19</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,10 +30,10 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="additional" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\jtshelby\Box Sync\iastate\DARCTeam\digitalCollections\github_resources\dataDictionary\additional.txt" tab="0" delimiter="|">
+  <connection id="1" name="excelAdditional" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\excelAdditional." delimiter="|">
       <textFields count="12">
-        <textField type="skip"/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -48,10 +48,10 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="core" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr sourceFile="C:\Users\jtshelby\Box Sync\iastate\DARCTeam\digitalCollections\github_resources\dataDictionary\core.txt" tab="0" delimiter="|">
+  <connection id="2" name="excelCore" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\excelCore." delimiter="|">
       <textFields count="12">
-        <textField type="skip"/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -396,7 +396,7 @@
     <t xml:space="preserve"> Select subject headings after performing subject analysis. Use LCSH or local controlled vocabulary as appropriate. Do not assign places, personal names, corporate names, events, or time periods to this field; instead, enter these in the `Geographic Subject`, `People`, `Organizations`, `Events`, and `Time Period` fields, respectively.  &lt;br&gt;&lt;br&gt;  Use information given in tables of contents within the resource as well as any notes on the object itself; however, it is not obligatory to perform more extensive research for subject analysis beyond what has been included. It is acceptable to include subject terms outside of the controlled vocabularies for the purpose of improving the user search experience. These values will be added to the local controlled vocabulary. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Photographs  &lt;br&gt;&lt;br&gt;  Agricultural engineering--Iowa  &lt;br&gt;&lt;br&gt;  Agricultural machinery                                                                                                                                                                                                                                                                                                                                                </t>
+    <t xml:space="preserve"> Photographs  &lt;br&gt;&lt;br&gt;  Agricultural engineering  &lt;br&gt;&lt;br&gt;  College students                                                                                                                                                                                                                                                                                                                                                            </t>
   </si>
   <si>
     <t xml:space="preserve"> Title                    </t>
@@ -654,10 +654,10 @@
     <t xml:space="preserve"> People                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> A person or type of person that is associated with a resource or that the resource is about.                                                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shreve, Earl; faculty                                                                                                                                                                                                                                                                                                                                                       </t>
+    <t xml:space="preserve"> A person that is associated with a resource or that the resource is about.                                                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shreve, Earl                                                                                                                                                                                                                                                                                                                                                                </t>
   </si>
   <si>
     <t xml:space="preserve"> Time Period            </t>
@@ -737,11 +737,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="core" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excelCore." connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="additional" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excelAdditional." connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1640,7 +1640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Removed "Campus scenes" and did some copy editing
</commit_message>
<xml_diff>
--- a/data dictionary/dataDictionary.xlsx
+++ b/data dictionary/dataDictionary.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="888" yWindow="0" windowWidth="22152" windowHeight="9396"/>
+    <workbookView xWindow="888" yWindow="0" windowWidth="22152" windowHeight="9396" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Core" sheetId="1" r:id="rId1"/>
-    <sheet name="Additional" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="excelAdditional." localSheetId="1">Additional!$A$1:$K$17</definedName>
-    <definedName name="excelCore." localSheetId="0">Core!$A$1:$K$19</definedName>
+    <definedName name="additional" localSheetId="1">Sheet2!$A$1:$K$16</definedName>
+    <definedName name="core" localSheetId="0">Core!$A$1:$K$19</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,8 +30,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="excelAdditional" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\excelAdditional." delimiter="|">
+  <connection id="1" name="additional" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\additional.txt" delimiter="|">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -48,8 +48,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="excelCore" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr sourceFile="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\excelCore." delimiter="|">
+  <connection id="2" name="core" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\jtshelby\Box Sync\iastate\groups\internal\DARCTeam\digitalCollections\github_resources\dataDictionary\core.txt" delimiter="|">
       <textFields count="12">
         <textField/>
         <textField/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="205">
   <si>
     <t xml:space="preserve"> Field label              </t>
   </si>
@@ -294,10 +294,13 @@
     <t xml:space="preserve"> Recommended       </t>
   </si>
   <si>
+    <t xml:space="preserve"> DC: "The size or duration of the resource."                                                                                                                                                                                       </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Use separate values for each aspect of extent recorded. For multi-page documents, include number of pages. For objects, include dimensions only if given and if they are relevant to the use of the collection. When recording dimensions, use the metric system. For sound or video resources, include time duration of recording.                                                                                                                                                                                                                                                                                                                                                                                                                                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> 200 pages  &lt;br&gt;&lt;br&gt;  4 photographs + handwritten notes  &lt;br&gt;&lt;br&gt;  24.2 x 25 cm                                                                                                                                                                                                                                                                                                                                                         </t>
+    <t xml:space="preserve"> 200 pages  &lt;br&gt;&lt;br&gt;  24.2 x 25 cm                                                                                                                                                                                                                                                                                                                                                                                                      </t>
   </si>
   <si>
     <t xml:space="preserve"> Format-Medium            </t>
@@ -309,6 +312,9 @@
     <t xml:space="preserve"> Local, derived from Getty AAT                                                                </t>
   </si>
   <si>
+    <t xml:space="preserve"> DC: "The material or physical carrier of the resource."                                                                                                                                                                           </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Describe the physical medium of the original (depicted or scanned) resource. Use the local controlled vocabulary which has been derived from the Art and Architecture Thesaurus (AAT), [http://www.getty.edu/research/tools/vocabularies/aat/](http://www.getty.edu/research/tools/vocabularies/aat/). This value should reflect a cultural heritage vocabulary for artifacts rather than an internet media or file type. Use the **preferred** term.                                                                                                                                                                                                                                                                                                                                               </t>
   </si>
   <si>
@@ -411,7 +417,7 @@
     <t xml:space="preserve"> Create a descriptive title for the item/object following the general guidelines for titles given in Describing Archives: a Content Standard (DACS) 2.3 Title (page 17).  &lt;br&gt;&lt;br&gt;  Prefer any information given within the resource itself, such as the authorâ€™s table of contents or a hand-written note on an album page serving the function of a title page. Information from the finding aid (see Appendix I) can,also be used to assist in item identification.   &lt;br&gt;&lt;br&gt;  For correspondence, follow the format: **[authorized name of sender] letter to [authorized name of recipient] regarding [subject], [date]**                                                                                                                                                                       </t>
   </si>
   <si>
-    <t xml:space="preserve"> J.B. Davidson pictorial record, trip to Europe (Germany, England, France, Spain), book 1 of 3 *[compound object based on hand-written note on title page]*  &lt;br&gt;&lt;br&gt;  J.B. Davidson notes, photographs, and proceedings documenting agricultural work in China, 1948-1949  &lt;br&gt;&lt;br&gt;  Page 6 *[page-level description of compound object]*                                                                                              </t>
+    <t xml:space="preserve"> J.B. Davidson pictorial record, trip to Europe (Germany, England, France, Spain), book 1 of 3 *[compound object based on hand-written note on title page]*  &lt;br&gt;&lt;br&gt;  Chemistry Building, circa 1910 *[photograph of a building]*  &lt;br&gt;&lt;br&gt;  Graduates walking across campus, 1906 *[photograph of an event]*                                                                                                                          </t>
   </si>
   <si>
     <t xml:space="preserve"> Type                     </t>
@@ -501,7 +507,10 @@
     <t xml:space="preserve"> #16. Jack Trice Plaza - 97 - 2606. Photo: K. Lyles. 8/07/97                                                                                                                                                                                                                                                                                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Campus Landmarks       </t>
+    <t xml:space="preserve"> Events                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dcterms:subject     </t>
   </si>
   <si>
     <t xml:space="preserve"> Used for faceting                       </t>
@@ -510,66 +519,60 @@
     <t xml:space="preserve"> Recommended if relevant </t>
   </si>
   <si>
+    <t xml:space="preserve"> LCSH, local                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> An event of which the resource is about.                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Use LCSH or local vocabulary terms when available.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Commencement ceremonies                                                                                                                                                                                                                                                                                                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cataloging &amp; Metadata Unit                                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Folder Title           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The name of the archival folder.                                                                                                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Central Campus]                                                                                                                                                                                                                                                                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Geographic Subject     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dcterms:spatial     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recommended             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Local, derived from Getty TGN, LCSH, or local resources </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DC Spatial Coverage: Spatial characteristics of the resource.                                                                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assign one or more geographic location(s) or subject(s) to the item. Consult the Getty Thesaurus of Geographic Names (TGN) ([http://www.getty.edu/research/tools/vocabularies/tgn/](http://www.getty.edu/research/tools/vocabularies/tgn/) ) for preferred names of geographic places. Choose the English-preferred (English-P) value if different from the overall preferred value. Give enough context that,the place information can be determined internationally (see examples).  &lt;br&gt;&lt;br&gt;  However, for local place names (ex: ISU campus), you may use LCSH if established term exists, or generate local controlled term. Use local controlled vocabulary to ensure consistency in location specific to campus and Ames. Follow local syntax and punctuation practices. List place strings hierarchically in ascending order of granularity (least specific to most specific) if using LCSH. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yangtze River *[use English-preferred values for places known in multiple languages]*  &lt;br&gt;&lt;br&gt;  Paris, France  &lt;br&gt;&lt;br&gt;  Chicago, Illinois  &lt;br&gt;&lt;br&gt;  Iowa State University  &lt;br&gt;&lt;br&gt;  Beardshear Hall (Ames, Iowa)                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hardware/Software      </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Local                                                   </t>
   </si>
   <si>
-    <t xml:space="preserve"> A local place associated with the resource or of which the resource is about.                                                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Use local vocabulary terms when available.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Campanile; Beardshear Hall                                                                                                                                                                                                                                                                                                                                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cataloging &amp; Metadata Unit                                                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Events                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> An event of which the resource is about.                                                                                                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Commencement                                                                                                                                                                                                                                                                                                                                                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Folder Title           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The name of the archival folder.                                                                                                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [Central Campus]                                                                                                                                                                                                                                                                                                                                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Geographic Subject     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dcterms:spatial     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Recommended             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Local, derived from Getty TGN, LCSH, or local resources </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DC Spatial Coverage: Spatial characteristics of the resource.                                                                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Assign one or more geographic location(s) or subject(s) to the item. Consult the Getty Thesaurus of Geographic Names (TGN) ([http://www.getty.edu/research/tools/vocabularies/tgn/](http://www.getty.edu/research/tools/vocabularies/tgn/) ) for preferred names of geographic places. Choose the English-preferred (English-P) value if different from the overall preferred value. Give enough context that,the place information can be determined internationally (see examples).  &lt;br&gt;&lt;br&gt;  However, for local place names (ex: ISU campus), you may use LCSH if established term exists, or generate local controlled term. Use local controlled vocabulary to ensure consistency in location specific to campus and Ames. Follow local syntax and punctuation practices. List place strings hierarchically in ascending order of granularity (least specific to most specific) if using LCSH. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yangtze River *[use English-preferred values for places known in multiple languages]*  &lt;br&gt;&lt;br&gt;  Paris, France  &lt;br&gt;&lt;br&gt;  Chicago, Illinois  &lt;br&gt;&lt;br&gt;  United States--Iowa--Ames--Iowa State University *[established LCSH heading, listed in local controlled vocabulary]*                                                                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hardware/Software      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> DC: "The method by which items are added to a collection."                                                                                                </t>
   </si>
   <si>
@@ -645,7 +648,10 @@
     <t xml:space="preserve"> Organizations          </t>
   </si>
   <si>
-    <t xml:space="preserve"> An organization that is in some way associated with the resource.                                                                                         </t>
+    <t xml:space="preserve"> An organization that is in some way associated with the resource.                                                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Use LCSH local vocabulary terms when available.                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                      </t>
   </si>
   <si>
     <t xml:space="preserve"> Iowa State University                                                                                                                                                                                                                                                                                                                                                       </t>
@@ -654,16 +660,13 @@
     <t xml:space="preserve"> People                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> A person that is associated with a resource or that the resource is about.                                                                                </t>
+    <t xml:space="preserve"> A person that is associated with a resource or that the resource is about.                                                                          </t>
   </si>
   <si>
     <t xml:space="preserve"> Shreve, Earl                                                                                                                                                                                                                                                                                                                                                                </t>
   </si>
   <si>
     <t xml:space="preserve"> Time Period            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dcterms:subject     </t>
   </si>
   <si>
     <t xml:space="preserve"> DC: "A point or period of time associated with an event in the lifecycle of the resource."                                                                </t>
@@ -737,11 +740,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excelCore." connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="core" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excelAdditional." connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="additional" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1009,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1363,13 +1366,13 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s">
         <v>40</v>
@@ -1377,10 +1380,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1392,16 +1395,16 @@
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J12" t="s">
         <v>40</v>
@@ -1409,10 +1412,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1424,16 +1427,16 @@
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J13" t="s">
         <v>19</v>
@@ -1441,13 +1444,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -1462,10 +1465,10 @@
         <v>45</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J14" t="s">
         <v>40</v>
@@ -1473,31 +1476,31 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J15" t="s">
         <v>40</v>
@@ -1505,10 +1508,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1523,13 +1526,13 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J16" t="s">
         <v>53</v>
@@ -1537,10 +1540,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1552,16 +1555,16 @@
         <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I17" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J17" t="s">
         <v>40</v>
@@ -1569,10 +1572,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1587,13 +1590,13 @@
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J18" t="s">
         <v>40</v>
@@ -1601,10 +1604,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1616,16 +1619,16 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J19" t="s">
         <v>40</v>
@@ -1638,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,546 +1661,514 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="I5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J5" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="J6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="G7" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="H7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="I7" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="J7" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="H8" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="I8" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="J8" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" t="s">
+        <v>180</v>
+      </c>
+      <c r="J9" t="s">
         <v>170</v>
-      </c>
-      <c r="B9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>133</v>
-      </c>
-      <c r="G9" t="s">
-        <v>173</v>
-      </c>
-      <c r="H9" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" t="s">
-        <v>175</v>
-      </c>
-      <c r="J9" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G10" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="J10" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G11" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I11" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="J11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G12" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="H12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="J12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="G13" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H13" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="I13" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="J13" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G14" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="I14" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="J14" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="G15" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="H15" t="s">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="I15" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="J15" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G16" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="H16" t="s">
-        <v>199</v>
+        <v>137</v>
       </c>
       <c r="I16" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="J16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>133</v>
-      </c>
-      <c r="G17" t="s">
-        <v>202</v>
-      </c>
-      <c r="H17" t="s">
-        <v>135</v>
-      </c>
-      <c r="I17" t="s">
-        <v>179</v>
-      </c>
-      <c r="J17" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>